<commit_message>
New data and attempt to functionize everything
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a-place-for-salvador-allende.xlsx
+++ b/a-place-for-salvador-allende/a-place-for-salvador-allende.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1578" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76AB5A1D-4637-4DA6-8AA9-E3B1495A5301}"/>
+  <xr:revisionPtr revIDLastSave="1605" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BEF3A34-5829-4D05-B313-B161C81218EB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="allende" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">allende!$B$1:$AO$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">allende!$B$1:$AO$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="748">
   <si>
     <t>id</t>
   </si>
@@ -2204,6 +2204,185 @@
   </si>
   <si>
     <t>https://www.openstreetmap.org/way/758217539</t>
+  </si>
+  <si>
+    <t>Salvador Allende street</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Sarajevo</t>
+  </si>
+  <si>
+    <t>Dobrinja</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/02/18/59-sarajevo-bosnia-herzegovina</t>
+  </si>
+  <si>
+    <t>Villa Salvador Allende</t>
+  </si>
+  <si>
+    <t>La Pintana</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NbqWJV69Cbu8h53k6</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/9728569027</t>
+  </si>
+  <si>
+    <t>Praça Salvador Allende</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Rio Grande do Sul</t>
+  </si>
+  <si>
+    <t>Porto Alegre</t>
+  </si>
+  <si>
+    <t>Centro Histórico</t>
+  </si>
+  <si>
+    <t>90050-200</t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Porto Alegre
+Secretaria Municipal do Meio Ambiente
+Praça Salvador Allende 
+Presidente chileno. Herói das Américas
+2013</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/305752671</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/4FGZmC5aXyT4RUSc9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2013/06/24/597-porto-alegre-brasil</t>
+  </si>
+  <si>
+    <t>Monumento al presidente Salvador Allende en Brasilia</t>
+  </si>
+  <si>
+    <t>Distrito Federal</t>
+  </si>
+  <si>
+    <t>Brasilia</t>
+  </si>
+  <si>
+    <t>Salvador Allende
+Tenho fé no Chile e no seu destino, sigam vocês sabendo que, muito mais cedo do que tarde, abrir-se-âo as grandes alamedas por onde passe o homem livre, para construir uma sociedade melhor.
+(Presidente Allende, 11 de setembro 1973)</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2011/12/12/550-brasilia-brasil</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>22783-020</t>
+  </si>
+  <si>
+    <t>Avenida Salvador Allende
+(1908 - 1973) Médico, fundador do Partido Socialista, presidente do Chile (1970-1973).</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/426694183</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/fakGRb84JRo2jQj8A</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/07/29/499-rio-de-janeiro-brasil</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>Sacomã</t>
+  </si>
+  <si>
+    <t>Vila das Mercês</t>
+  </si>
+  <si>
+    <t>04165-000</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/292191474</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/oCKr4cgZmgq7mkCQ6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/12/08/291-sao-paulo-brasil</t>
+  </si>
+  <si>
+    <t>Salvador Allende Bus Station</t>
+  </si>
+  <si>
+    <t>public transport station</t>
+  </si>
+  <si>
+    <t>Recreio dos Bandeirantes</t>
+  </si>
+  <si>
+    <t>Avenida das Américas</t>
+  </si>
+  <si>
+    <t>22790-710</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/276421960</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/hfjxEk8grbHLu8239</t>
+  </si>
+  <si>
+    <t>бул. „Андрей Сахаров“ / Boulevard "Andrej Sakharov"</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Sofia City Province</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Mladost</t>
+  </si>
+  <si>
+    <t>Mladost 1</t>
+  </si>
+  <si>
+    <t>Salvador Allende, 1908-1973, hijo ilustre del pueblo chileno
+Entregó su vida por la causa de la paz, la democracia y el progreso socialista</t>
+  </si>
+  <si>
+    <t>bg</t>
+  </si>
+  <si>
+    <t>бул. „Салвадор Алиенде“ / Boulevard "Salvador Allende"</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/69596345</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/LfxjeoGtcJmf8gm16</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/10/02/110-sofia-bulgaria</t>
   </si>
 </sst>
 </file>
@@ -2534,13 +2713,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AO119"/>
+  <dimension ref="A1:AO127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A120" sqref="A120"/>
+      <selection pane="bottomRight" activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10203,8 +10382,450 @@
         <v>690</v>
       </c>
     </row>
+    <row r="120" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="3">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="N120" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O120" s="3">
+        <v>2</v>
+      </c>
+      <c r="P120" s="3">
+        <v>18</v>
+      </c>
+      <c r="V120" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="3" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="121" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="3">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="K121" s="10">
+        <v>8010000</v>
+      </c>
+      <c r="L121" s="3">
+        <v>-33.580694899999997</v>
+      </c>
+      <c r="M121" s="3">
+        <v>-70.646144500000005</v>
+      </c>
+      <c r="N121" s="3">
+        <v>2012</v>
+      </c>
+      <c r="O121" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q121" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V121" s="3">
+        <v>1</v>
+      </c>
+      <c r="W121" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="X121" s="3" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="122" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="3">
+        <v>121</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="K122" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="L122" s="3">
+        <v>-30.034959675270098</v>
+      </c>
+      <c r="M122" s="3">
+        <v>-51.223894258388903</v>
+      </c>
+      <c r="N122" s="3">
+        <v>2004</v>
+      </c>
+      <c r="O122" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q122" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="V122" s="3">
+        <v>1</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="Y122" s="3" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="3">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="N123" s="3">
+        <v>2008</v>
+      </c>
+      <c r="Q123" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="R123" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="S123" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="V123" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y123" s="3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="124" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="3">
+        <v>123</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="K124" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="L124" s="3">
+        <v>-22.985492037936801</v>
+      </c>
+      <c r="M124" s="3">
+        <v>-43.413389967982098</v>
+      </c>
+      <c r="N124" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O124" s="3">
+        <v>2</v>
+      </c>
+      <c r="P124" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q124" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="V124" s="3">
+        <v>1</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="Y124" s="3" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="125" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="3">
+        <v>124</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="K125" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="L125" s="3">
+        <v>-23.618749999999999</v>
+      </c>
+      <c r="M125" s="3">
+        <v>-46.610177</v>
+      </c>
+      <c r="N125" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O125" s="3">
+        <v>2</v>
+      </c>
+      <c r="P125" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q125" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="V125" s="3">
+        <v>1</v>
+      </c>
+      <c r="W125" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="X125" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="Y125" s="3" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="126" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="3">
+        <v>125</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="K126" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="L126" s="3">
+        <v>-23.0082369008645</v>
+      </c>
+      <c r="M126" s="3">
+        <v>-43.442585473568698</v>
+      </c>
+      <c r="N126" s="3">
+        <v>2014</v>
+      </c>
+      <c r="O126" s="3">
+        <v>4</v>
+      </c>
+      <c r="P126" s="3">
+        <v>22</v>
+      </c>
+      <c r="Q126" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="V126" s="3">
+        <v>1</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="127" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="3">
+        <v>126</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="K127" s="10">
+        <v>1729</v>
+      </c>
+      <c r="L127" s="3">
+        <v>42.652000000000001</v>
+      </c>
+      <c r="M127" s="3">
+        <v>23.37491</v>
+      </c>
+      <c r="N127" s="3">
+        <v>1977</v>
+      </c>
+      <c r="Q127" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="R127" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="S127" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="U127" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="V127" s="3">
+        <v>1</v>
+      </c>
+      <c r="W127" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="X127" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="Y127" s="3" t="s">
+        <v>747</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:AO107" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:AO127" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reorganize old test scripts
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a-place-for-salvador-allende.xlsx
+++ b/a-place-for-salvador-allende/a-place-for-salvador-allende.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1638" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34EA4910-C6DE-4A8A-A3B3-BA87244E3EFE}"/>
+  <xr:revisionPtr revIDLastSave="1646" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{353E9B1F-0C10-41B3-98AB-1F19707E6000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allende" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">allende!$B$1:$AO$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">allende!$B$1:$AO$148</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3166,7 +3166,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A149" sqref="A149"/>
+      <selection pane="bottomRight" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12478,7 +12478,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AO136" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:AO148" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>